<commit_message>
Adicionado instalador do gerenciador
</commit_message>
<xml_diff>
--- a/cmc/docs/cpo05_AssignedKeys.xlsx
+++ b/cmc/docs/cpo05_AssignedKeys.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\colibri-extensions\cmc\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5B5F186E-3FB6-4251-A1BA-7381BEEFEF8E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19665" windowHeight="10950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19665" windowHeight="10950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,18 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>pitty home</t>
   </si>
   <si>
     <t>pitty note NCR</t>
   </si>
+  <si>
+    <t>pitty desk NCR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -384,11 +386,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,6 +418,9 @@
       <c r="A3">
         <v>1088002</v>
       </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1437,5 +1442,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>